<commit_message>
Add half of the functions
</commit_message>
<xml_diff>
--- a/inst/extdata/input/cd_sheet.xlsx
+++ b/inst/extdata/input/cd_sheet.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5CA49A-7384-4589-8776-49B683525A74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8C310-36BE-4E02-A27D-9C31DD3E1F76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="1040" windowWidth="9320" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="5" r:id="rId1"/>
-    <sheet name="description" sheetId="4" r:id="rId2"/>
-    <sheet name="distributions" sheetId="2" r:id="rId3"/>
+    <sheet name="additional_infos" sheetId="2" r:id="rId2"/>
+    <sheet name="description" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="101">
   <si>
     <t>see the sheets "Parameters" and "Distributions"</t>
   </si>
@@ -84,9 +84,6 @@
     <t>K_H</t>
   </si>
   <si>
-    <t>Degradability</t>
-  </si>
-  <si>
     <t>D_air</t>
   </si>
   <si>
@@ -213,27 +210,15 @@
     <t>m³/m³</t>
   </si>
   <si>
-    <t>c_pH</t>
-  </si>
-  <si>
-    <t>c_oc</t>
-  </si>
-  <si>
     <t>pH - coefficient</t>
   </si>
   <si>
     <t>organic carbon coefficient</t>
   </si>
   <si>
-    <t>log_K</t>
-  </si>
-  <si>
     <t>normal</t>
   </si>
   <si>
-    <t>case</t>
-  </si>
-  <si>
     <t>logarithmic constant</t>
   </si>
   <si>
@@ -243,24 +228,9 @@
     <t>[µg/d]</t>
   </si>
   <si>
-    <t>c_c</t>
-  </si>
-  <si>
     <t>concentration coefficient</t>
   </si>
   <si>
-    <t>log_BCF</t>
-  </si>
-  <si>
-    <t>c_pH_BCF</t>
-  </si>
-  <si>
-    <t>c_c_BCF</t>
-  </si>
-  <si>
-    <t>c_oc_BCF</t>
-  </si>
-  <si>
     <t>c_fert</t>
   </si>
   <si>
@@ -301,6 +271,60 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>const_K_d</t>
+  </si>
+  <si>
+    <t>beta_c</t>
+  </si>
+  <si>
+    <t>beta_pH</t>
+  </si>
+  <si>
+    <t>beta_oc</t>
+  </si>
+  <si>
+    <t>const_BCF</t>
+  </si>
+  <si>
+    <t>gamma_c</t>
+  </si>
+  <si>
+    <t>gamma_pH</t>
+  </si>
+  <si>
+    <t>gamma_oc</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Kd_regType</t>
+  </si>
+  <si>
+    <t>indirect</t>
+  </si>
+  <si>
+    <t>polltant type</t>
+  </si>
+  <si>
+    <t>inorganic</t>
+  </si>
+  <si>
+    <t>"organic" or "inorganic"</t>
+  </si>
+  <si>
+    <t>Estimation of Kd by log linear regression: Either "direct" , "indirect" or "no"</t>
+  </si>
+  <si>
+    <t>BCF_regType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation of BCF by log linear regression: Either "direct" or "indirect" </t>
   </si>
 </sst>
 </file>
@@ -1472,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6E1683-D001-49B1-A843-7E986734A50F}">
-  <dimension ref="A1:BY155"/>
+  <dimension ref="A1:BY154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1495,34 +1519,34 @@
   <sheetData>
     <row r="1" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:77" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1530,10 +1554,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="34">
         <v>0</v>
@@ -1546,7 +1570,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="16"/>
@@ -1623,10 +1647,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>6</v>
@@ -1639,7 +1663,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="16"/>
@@ -1716,10 +1740,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="34">
         <v>0</v>
@@ -1732,7 +1756,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="16"/>
@@ -1809,10 +1833,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>6</v>
@@ -1825,7 +1849,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="16"/>
@@ -1902,10 +1926,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>6</v>
@@ -1918,7 +1942,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="16"/>
@@ -1995,10 +2019,10 @@
         <v>19</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="18">
         <v>0</v>
@@ -2011,7 +2035,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="19"/>
@@ -2088,10 +2112,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>6</v>
@@ -2104,7 +2128,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="19"/>
@@ -2181,10 +2205,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>6</v>
@@ -2197,7 +2221,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="19"/>
@@ -2274,10 +2298,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>6</v>
@@ -2290,7 +2314,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="19"/>
@@ -2364,13 +2388,13 @@
     </row>
     <row r="11" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>6</v>
@@ -2383,7 +2407,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="19"/>
@@ -2457,13 +2481,13 @@
     </row>
     <row r="12" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>6</v>
@@ -2476,7 +2500,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="19"/>
@@ -2550,14 +2574,12 @@
     </row>
     <row r="13" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>5</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C13" s="19"/>
       <c r="D13" s="18" t="s">
         <v>6</v>
       </c>
@@ -2569,7 +2591,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="19"/>
@@ -2641,29 +2663,31 @@
       <c r="BX13" s="55"/>
       <c r="BY13" s="55"/>
     </row>
-    <row r="14" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9">
         <v>0</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="19"/>
+      <c r="H14" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="55"/>
       <c r="L14" s="55"/>
       <c r="M14" s="55"/>
@@ -2734,26 +2758,28 @@
     </row>
     <row r="15" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="D15" s="20">
+        <v>3.42</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.11</v>
+      </c>
       <c r="F15" s="9">
         <v>0</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H15" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="21"/>
@@ -2827,28 +2853,28 @@
     </row>
     <row r="16" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="20">
-        <v>3.42</v>
+        <v>1.08</v>
       </c>
       <c r="E16" s="9">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="F16" s="9">
         <v>0</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H16" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="21"/>
@@ -2922,16 +2948,16 @@
     </row>
     <row r="17" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="20">
-        <v>1.08</v>
+        <v>-0.47</v>
       </c>
       <c r="E17" s="9">
         <v>0.02</v>
@@ -2940,10 +2966,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="21"/>
@@ -3017,28 +3043,28 @@
     </row>
     <row r="18" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>63</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>65</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="20">
-        <v>-0.47</v>
+        <v>-0.81</v>
       </c>
       <c r="E18" s="9">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="F18" s="9">
         <v>0</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H18" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="21"/>
@@ -3110,33 +3136,31 @@
       <c r="BX18" s="55"/>
       <c r="BY18" s="55"/>
     </row>
-    <row r="19" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="20">
-        <v>-0.81</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="F19" s="9">
+    <row r="19" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4">
         <v>0</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="21"/>
+      <c r="G19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="55"/>
       <c r="L19" s="55"/>
       <c r="M19" s="55"/>
@@ -3213,7 +3237,7 @@
         <v>54</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>6</v>
@@ -3226,7 +3250,7 @@
         <v>7</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="19"/>
@@ -3298,31 +3322,31 @@
       <c r="BX20" s="55"/>
       <c r="BY20" s="55"/>
     </row>
-    <row r="21" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="49" t="s">
+    <row r="21" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9">
         <v>0</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="19"/>
+      <c r="H21" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
       <c r="M21" s="55"/>
@@ -3393,16 +3417,16 @@
     </row>
     <row r="22" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>6</v>
+      <c r="D22" s="33">
+        <v>0.35</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9">
@@ -3412,7 +3436,7 @@
         <v>7</v>
       </c>
       <c r="H22" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="21"/>
@@ -3486,16 +3510,16 @@
     </row>
     <row r="23" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="33">
-        <v>0.35</v>
+        <v>0.76</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9">
@@ -3505,7 +3529,7 @@
         <v>7</v>
       </c>
       <c r="H23" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="21"/>
@@ -3579,16 +3603,16 @@
     </row>
     <row r="24" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="33">
-        <v>0.76</v>
+        <v>-0.15</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9">
@@ -3598,7 +3622,7 @@
         <v>7</v>
       </c>
       <c r="H24" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="21"/>
@@ -3672,16 +3696,16 @@
     </row>
     <row r="25" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="33">
-        <v>-0.15</v>
+        <v>-0.39</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9">
@@ -3691,7 +3715,7 @@
         <v>7</v>
       </c>
       <c r="H25" s="43" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="21"/>
@@ -3763,31 +3787,33 @@
       <c r="BX25" s="55"/>
       <c r="BY25" s="55"/>
     </row>
-    <row r="26" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="33">
-        <v>-0.39</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+    <row r="26" spans="1:77" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="35">
+        <v>-2.0824150533029799</v>
+      </c>
+      <c r="E26" s="36">
+        <v>0.56269971427805399</v>
+      </c>
+      <c r="F26" s="6">
         <v>0</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="21"/>
+      <c r="G26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="23"/>
       <c r="K26" s="55"/>
       <c r="L26" s="55"/>
       <c r="M26" s="55"/>
@@ -3858,28 +3884,26 @@
     </row>
     <row r="27" spans="1:77" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="35">
-        <v>-2.0824150533029799</v>
-      </c>
-      <c r="E27" s="36">
-        <v>0.56269971427805399</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="38"/>
       <c r="F27" s="6">
         <v>0</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="23"/>
@@ -3953,26 +3977,28 @@
     </row>
     <row r="28" spans="1:77" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="38"/>
+        <v>28</v>
+      </c>
+      <c r="D28" s="35">
+        <v>-14.429500000000001</v>
+      </c>
+      <c r="E28" s="36">
+        <v>0.79484520000000003</v>
+      </c>
       <c r="F28" s="6">
         <v>0</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="23"/>
@@ -4044,33 +4070,33 @@
       <c r="BX28" s="55"/>
       <c r="BY28" s="55"/>
     </row>
-    <row r="29" spans="1:77" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="35">
-        <v>-14.429500000000001</v>
-      </c>
-      <c r="E29" s="36">
-        <v>0.79484520000000003</v>
-      </c>
-      <c r="F29" s="6">
+    <row r="29" spans="1:77" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="E29" s="40">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F29" s="11">
         <v>0</v>
       </c>
-      <c r="G29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H29" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="23"/>
+      <c r="G29" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="24"/>
       <c r="K29" s="55"/>
       <c r="L29" s="55"/>
       <c r="M29" s="55"/>
@@ -4139,33 +4165,31 @@
       <c r="BX29" s="55"/>
       <c r="BY29" s="55"/>
     </row>
-    <row r="30" spans="1:77" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="39">
-        <v>0.9</v>
-      </c>
-      <c r="E30" s="40">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F30" s="11">
+    <row r="30" spans="1:77" s="31" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="25">
+        <v>58</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7">
         <v>0</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="24"/>
+      <c r="G30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="26"/>
       <c r="K30" s="55"/>
       <c r="L30" s="55"/>
       <c r="M30" s="55"/>
@@ -4239,13 +4263,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="D31" s="25">
-        <v>58</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7">
@@ -4327,31 +4351,31 @@
       <c r="BX31" s="55"/>
       <c r="BY31" s="55"/>
     </row>
-    <row r="32" spans="1:77" s="31" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="25" t="s">
+    <row r="32" spans="1:77" s="31" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="25">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7">
+      <c r="D32" s="27">
+        <v>0.3</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28">
         <v>0</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="46" t="s">
+      <c r="H32" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="26"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="29"/>
       <c r="K32" s="55"/>
       <c r="L32" s="55"/>
       <c r="M32" s="55"/>
@@ -4420,114 +4444,22 @@
       <c r="BX32" s="55"/>
       <c r="BY32" s="55"/>
     </row>
-    <row r="33" spans="1:77" s="31" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28">
-        <v>0</v>
-      </c>
-      <c r="G33" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="55"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
-      <c r="T33" s="55"/>
-      <c r="U33" s="55"/>
-      <c r="V33" s="55"/>
-      <c r="W33" s="55"/>
-      <c r="X33" s="55"/>
-      <c r="Y33" s="55"/>
-      <c r="Z33" s="55"/>
-      <c r="AA33" s="55"/>
-      <c r="AB33" s="55"/>
-      <c r="AC33" s="55"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="55"/>
-      <c r="AG33" s="55"/>
-      <c r="AH33" s="55"/>
-      <c r="AI33" s="55"/>
-      <c r="AJ33" s="55"/>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="55"/>
-      <c r="AM33" s="55"/>
-      <c r="AN33" s="55"/>
-      <c r="AO33" s="55"/>
-      <c r="AP33" s="55"/>
-      <c r="AQ33" s="55"/>
-      <c r="AR33" s="55"/>
-      <c r="AS33" s="55"/>
-      <c r="AT33" s="55"/>
-      <c r="AU33" s="55"/>
-      <c r="AV33" s="55"/>
-      <c r="AW33" s="55"/>
-      <c r="AX33" s="55"/>
-      <c r="AY33" s="55"/>
-      <c r="AZ33" s="55"/>
-      <c r="BA33" s="55"/>
-      <c r="BB33" s="55"/>
-      <c r="BC33" s="55"/>
-      <c r="BD33" s="55"/>
-      <c r="BE33" s="55"/>
-      <c r="BF33" s="55"/>
-      <c r="BG33" s="55"/>
-      <c r="BH33" s="55"/>
-      <c r="BI33" s="55"/>
-      <c r="BJ33" s="55"/>
-      <c r="BK33" s="55"/>
-      <c r="BL33" s="55"/>
-      <c r="BM33" s="55"/>
-      <c r="BN33" s="55"/>
-      <c r="BO33" s="55"/>
-      <c r="BP33" s="55"/>
-      <c r="BQ33" s="55"/>
-      <c r="BR33" s="55"/>
-      <c r="BS33" s="55"/>
-      <c r="BT33" s="55"/>
-      <c r="BU33" s="55"/>
-      <c r="BV33" s="55"/>
-      <c r="BW33" s="55"/>
-      <c r="BX33" s="55"/>
-      <c r="BY33" s="55"/>
-    </row>
-    <row r="34" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:77" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="33" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="34" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="35" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="37" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="41" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="43" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="48" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="49" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="50" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="51" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -4634,13 +4566,75 @@
     <row r="152" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="153" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="154" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="155" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="70.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -4663,18 +4657,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add all functions for table preperation
</commit_message>
<xml_diff>
--- a/inst/extdata/input/cd_sheet.xlsx
+++ b/inst/extdata/input/cd_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8C310-36BE-4E02-A27D-9C31DD3E1F76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076A5050-CC59-4770-98A0-9D47DAB57AB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="1040" windowWidth="9320" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
   <si>
     <t>see the sheets "Parameters" and "Distributions"</t>
   </si>
@@ -114,12 +114,6 @@
     <t>PNEC_human</t>
   </si>
   <si>
-    <t>PNEC_organisms</t>
-  </si>
-  <si>
-    <t>PNEC_leachate</t>
-  </si>
-  <si>
     <t>vapour pressure</t>
   </si>
   <si>
@@ -325,6 +319,18 @@
   </si>
   <si>
     <t xml:space="preserve">Estimation of BCF by log linear regression: Either "direct" or "indirect" </t>
+  </si>
+  <si>
+    <t>PNEC_water</t>
+  </si>
+  <si>
+    <t>PNEC_water_type</t>
+  </si>
+  <si>
+    <t>Specifitaion of the water type: "groundwater", "surface water" or "see water"</t>
+  </si>
+  <si>
+    <t>PNEC_soil</t>
   </si>
 </sst>
 </file>
@@ -1498,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6E1683-D001-49B1-A843-7E986734A50F}">
   <dimension ref="A1:BY154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,34 +1525,34 @@
   <sheetData>
     <row r="1" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>81</v>
-      </c>
       <c r="J1" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:77" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1554,7 +1560,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>21</v>
@@ -1570,7 +1576,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="16"/>
@@ -1647,7 +1653,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>21</v>
@@ -1663,7 +1669,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="16"/>
@@ -1740,7 +1746,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>21</v>
@@ -1756,7 +1762,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="16"/>
@@ -1833,7 +1839,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
@@ -1849,7 +1855,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="16"/>
@@ -1926,7 +1932,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>21</v>
@@ -1942,7 +1948,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="16"/>
@@ -2019,7 +2025,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>27</v>
@@ -2035,7 +2041,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="19"/>
@@ -2112,7 +2118,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>23</v>
@@ -2128,7 +2134,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="19"/>
@@ -2205,7 +2211,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>24</v>
@@ -2221,7 +2227,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="19"/>
@@ -2298,7 +2304,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>25</v>
@@ -2314,7 +2320,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="19"/>
@@ -2391,7 +2397,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>2</v>
@@ -2407,7 +2413,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="19"/>
@@ -2484,7 +2490,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>5</v>
@@ -2500,7 +2506,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="19"/>
@@ -2574,10 +2580,10 @@
     </row>
     <row r="13" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="18" t="s">
@@ -2591,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="19"/>
@@ -2665,10 +2671,10 @@
     </row>
     <row r="14" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>5</v>
@@ -2684,7 +2690,7 @@
         <v>7</v>
       </c>
       <c r="H14" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="21"/>
@@ -2758,10 +2764,10 @@
     </row>
     <row r="15" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>3</v>
@@ -2776,10 +2782,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H15" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="21"/>
@@ -2853,10 +2859,10 @@
     </row>
     <row r="16" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>3</v>
@@ -2871,10 +2877,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H16" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="21"/>
@@ -2948,10 +2954,10 @@
     </row>
     <row r="17" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>3</v>
@@ -2966,10 +2972,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="21"/>
@@ -3043,10 +3049,10 @@
     </row>
     <row r="18" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>3</v>
@@ -3061,10 +3067,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H18" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="21"/>
@@ -3138,13 +3144,13 @@
     </row>
     <row r="19" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="49" t="s">
-        <v>53</v>
-      </c>
       <c r="C19" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>6</v>
@@ -3157,7 +3163,7 @@
         <v>7</v>
       </c>
       <c r="H19" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="19"/>
@@ -3231,13 +3237,13 @@
     </row>
     <row r="20" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>6</v>
@@ -3250,7 +3256,7 @@
         <v>7</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="19"/>
@@ -3327,7 +3333,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>3</v>
@@ -3343,7 +3349,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="21"/>
@@ -3417,10 +3423,10 @@
     </row>
     <row r="22" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>3</v>
@@ -3436,7 +3442,7 @@
         <v>7</v>
       </c>
       <c r="H22" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="21"/>
@@ -3510,10 +3516,10 @@
     </row>
     <row r="23" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>3</v>
@@ -3529,7 +3535,7 @@
         <v>7</v>
       </c>
       <c r="H23" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="21"/>
@@ -3603,10 +3609,10 @@
     </row>
     <row r="24" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>3</v>
@@ -3622,7 +3628,7 @@
         <v>7</v>
       </c>
       <c r="H24" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="21"/>
@@ -3696,10 +3702,10 @@
     </row>
     <row r="25" spans="1:77" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>3</v>
@@ -3715,7 +3721,7 @@
         <v>7</v>
       </c>
       <c r="H25" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="21"/>
@@ -3789,10 +3795,10 @@
     </row>
     <row r="26" spans="1:77" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="23" t="s">
         <v>26</v>
@@ -3807,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H26" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="23"/>
@@ -3887,7 +3893,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="23" t="s">
         <v>22</v>
@@ -3903,7 +3909,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="23"/>
@@ -3980,7 +3986,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" s="23" t="s">
         <v>28</v>
@@ -3995,10 +4001,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="23"/>
@@ -4072,10 +4078,10 @@
     </row>
     <row r="29" spans="1:77" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B29" s="52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>26</v>
@@ -4090,10 +4096,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H29" s="45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="24"/>
@@ -4170,10 +4176,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="25">
         <v>58</v>
@@ -4260,13 +4266,13 @@
     </row>
     <row r="31" spans="1:77" s="31" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D31" s="25">
         <v>1.1499999999999999</v>
@@ -4353,13 +4359,13 @@
     </row>
     <row r="32" spans="1:77" s="31" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="27" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="B32" s="54" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="27">
         <v>0.3</v>
@@ -4573,10 +4579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4587,46 +4593,54 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
         <v>95</v>
       </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="C4" t="s">
-        <v>94</v>
+      <c r="B5" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>